<commit_message>
Re #1 and #16 adjustments made
</commit_message>
<xml_diff>
--- a/code-check.xlsx
+++ b/code-check.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t xml:space="preserve">Bureau of Labor Statistics' Quarterly Census of Employment and Wages </t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Effect of Labor Demand on Unemployment Receipt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qcew/regressions_table.do</t>
   </si>
   <si>
     <t xml:space="preserve">tables/table_bartik.tex</t>
@@ -317,8 +320,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,15 +376,15 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -399,341 +406,344 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="28.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="6.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.02"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="2" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="E22" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>62</v>
+      <c r="E25" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="E26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="C26" s="7"/>
+      <c r="E26" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="B27" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
+      <c r="A28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest update to README and data citations
</commit_message>
<xml_diff>
--- a/code-check.xlsx
+++ b/code-check.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t xml:space="preserve">Data Preparation Program</t>
   </si>
@@ -58,7 +58,16 @@
     <t xml:space="preserve">Creates the 1000 realizations of Czs</t>
   </si>
   <si>
-    <t xml:space="preserve">bootclusters_jtw1990_moe.sas7bdat, bootclusters_jtw1990_moe_new.dta</t>
+    <t xml:space="preserve">flows_jtw1990_moe.sas7bdat bootclusters_jtw1990_moe.sas7bdat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05_03_export_bootstraps.sas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exports data and does some stats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bootclusters_jtw1990_moe.csv, bootclusters_jtw1990_moe_new.dta, flows_jtw1990_moe.dta, flows_jtw1990_moe.csv</t>
   </si>
   <si>
     <t xml:space="preserve">06_qcew/00*do</t>
@@ -389,10 +398,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -449,7 +458,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -461,74 +470,72 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="D6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -540,24 +547,24 @@
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="9" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>34</v>
@@ -570,47 +577,47 @@
       <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="9" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>48</v>
@@ -624,76 +631,76 @@
         <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="9" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="1" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="9" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="9" t="s">
         <v>70</v>
       </c>
     </row>
@@ -701,20 +708,31 @@
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="2" t="s">
         <v>72</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="9"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="9"/>
@@ -726,14 +744,17 @@
       <c r="B30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="3"/>
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>